<commit_message>
filled in og data vals
</commit_message>
<xml_diff>
--- a/eval_data.xlsx
+++ b/eval_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhita/Documents/0Princeton/1_SophomoreYear/COS435/FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhita/Documents/0Princeton/1_SophomoreYear/COS435/COS435_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT56" workbookViewId="0">
-      <selection activeCell="AV88" sqref="AV88:AZ89"/>
+    <sheetView tabSelected="1" topLeftCell="AT60" workbookViewId="0">
+      <selection activeCell="AV76" sqref="AV76:AZ76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,20 +879,95 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G4">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="L4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M4">
+        <v>0.5</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>15.0501008584</v>
+      </c>
+      <c r="P4">
+        <v>1.4634528678300001</v>
+      </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AD4">
+        <v>0.95</v>
+      </c>
+      <c r="AE4">
+        <v>0.86363636363600005</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>30.053242021599999</v>
+      </c>
+      <c r="AH4">
+        <v>1.46345872806</v>
+      </c>
       <c r="AK4" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="AM4">
+        <v>0.25</v>
+      </c>
+      <c r="AN4">
+        <v>0.22727272727299999</v>
+      </c>
+      <c r="AO4">
+        <v>0.25</v>
+      </c>
+      <c r="AP4">
+        <v>1.53157201951</v>
+      </c>
+      <c r="AQ4">
+        <v>1.8221378548699999E-2</v>
+      </c>
       <c r="AT4" s="1" t="s">
         <v>62</v>
+      </c>
+      <c r="AV4">
+        <v>0.15</v>
+      </c>
+      <c r="AW4">
+        <v>0.13636363636400001</v>
+      </c>
+      <c r="AX4">
+        <v>0.125</v>
+      </c>
+      <c r="AY4">
+        <v>0.82142290159599995</v>
+      </c>
+      <c r="AZ4">
+        <v>8.0868675595200008E-3</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.2">
@@ -2329,20 +2404,95 @@
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C18">
+        <v>0.75</v>
+      </c>
+      <c r="D18">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G18">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="L18">
+        <v>0.7</v>
+      </c>
+      <c r="M18">
+        <v>0.63636363636399995</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>8.2244342271100006</v>
+      </c>
+      <c r="P18">
+        <v>0.38266054708199998</v>
+      </c>
       <c r="S18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="AB18" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>0.90909090909099999</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>7.0402683819199998</v>
+      </c>
+      <c r="AH18">
+        <v>0.100718798328</v>
+      </c>
       <c r="AK18" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="AM18">
+        <v>0.57894736842100003</v>
+      </c>
+      <c r="AN18">
+        <v>0.5</v>
+      </c>
+      <c r="AO18">
+        <v>0.33333333333300003</v>
+      </c>
+      <c r="AP18">
+        <v>13.478512328500001</v>
+      </c>
+      <c r="AQ18">
+        <v>0.34180626494100003</v>
+      </c>
       <c r="AT18" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="AV18">
+        <v>0.2</v>
+      </c>
+      <c r="AW18">
+        <v>0.181818181818</v>
+      </c>
+      <c r="AX18">
+        <v>0.111111111111</v>
+      </c>
+      <c r="AY18">
+        <v>1.0424588298199999</v>
+      </c>
+      <c r="AZ18">
+        <v>9.2154605551899998E-3</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.2">
@@ -3835,20 +3985,110 @@
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C33">
+        <v>0.75</v>
+      </c>
+      <c r="D33">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G33">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="J33" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="L33">
+        <v>0.25</v>
+      </c>
+      <c r="M33">
+        <v>0.22727272727299999</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>9.4721781331700008</v>
+      </c>
+      <c r="P33">
+        <v>0.45346406300999997</v>
+      </c>
       <c r="S33" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="U33">
+        <v>0.3</v>
+      </c>
+      <c r="V33">
+        <v>0.31276583899999999</v>
+      </c>
+      <c r="W33">
+        <v>0.5</v>
+      </c>
+      <c r="X33">
+        <v>4.5673298200000003</v>
+      </c>
+      <c r="Y33">
+        <v>0.56203285319999996</v>
+      </c>
       <c r="AB33" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AD33">
+        <v>0.7</v>
+      </c>
+      <c r="AE33">
+        <v>0.63636363636399995</v>
+      </c>
+      <c r="AF33">
+        <v>1</v>
+      </c>
+      <c r="AG33">
+        <v>21.391061511299998</v>
+      </c>
+      <c r="AH33">
+        <v>1.46345872806</v>
+      </c>
       <c r="AK33" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="AM33">
+        <v>0.5</v>
+      </c>
+      <c r="AN33">
+        <v>0.45454545454500001</v>
+      </c>
+      <c r="AO33">
+        <v>0.33333333333300003</v>
+      </c>
+      <c r="AP33">
+        <v>5.0566816920299997</v>
+      </c>
+      <c r="AQ33">
+        <v>0.32370127735600002</v>
+      </c>
       <c r="AT33" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="AV33">
+        <v>0.05</v>
+      </c>
+      <c r="AW33">
+        <v>4.5454545454499999E-2</v>
+      </c>
+      <c r="AX33">
+        <v>8.3333333333299994E-2</v>
+      </c>
+      <c r="AY33">
+        <v>0.270238154427</v>
+      </c>
+      <c r="AZ33">
+        <v>2.6041666666699998E-3</v>
       </c>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.2">
@@ -4626,19 +4866,19 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>0.05</v>
+        <v>0.75</v>
       </c>
       <c r="D41">
-        <v>4.5454545454499999E-2</v>
+        <v>0.68181818181800002</v>
       </c>
       <c r="E41">
-        <v>6.66666666667E-2</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>0.25</v>
+        <v>22.399506517700001</v>
       </c>
       <c r="G41">
-        <v>2.08333333333E-3</v>
+        <v>1.4634587241399999</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>6</v>
@@ -5285,17 +5525,92 @@
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C47">
+        <v>0.75</v>
+      </c>
+      <c r="D47">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G47">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="S47" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="U47">
+        <v>0.85</v>
+      </c>
+      <c r="V47">
+        <v>0.77272727272700004</v>
+      </c>
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47">
+        <v>25.379035872799999</v>
+      </c>
+      <c r="Y47">
+        <v>1.4634587241699999</v>
+      </c>
       <c r="AB47" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="AD47">
+        <v>0.65</v>
+      </c>
+      <c r="AE47">
+        <v>0.59090909090900001</v>
+      </c>
+      <c r="AF47">
+        <v>1</v>
+      </c>
+      <c r="AG47">
+        <v>21.0900315156</v>
+      </c>
+      <c r="AH47">
+        <v>1.46345872806</v>
+      </c>
       <c r="AK47" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="AM47">
+        <v>0.95</v>
+      </c>
+      <c r="AN47">
+        <v>0.86363636363600005</v>
+      </c>
+      <c r="AO47">
+        <v>1</v>
+      </c>
+      <c r="AP47">
+        <v>28.134479678000002</v>
+      </c>
+      <c r="AQ47">
+        <v>1.46345872806</v>
+      </c>
       <c r="AT47" s="1" t="s">
         <v>68</v>
+      </c>
+      <c r="AV47">
+        <v>0.05</v>
+      </c>
+      <c r="AW47">
+        <v>4.5454545454499999E-2</v>
+      </c>
+      <c r="AX47">
+        <v>8.3333333333299994E-2</v>
+      </c>
+      <c r="AY47">
+        <v>0.270238154427</v>
+      </c>
+      <c r="AZ47">
+        <v>2.6041666666699998E-3</v>
       </c>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.2">
@@ -5579,19 +5894,19 @@
         <v>3</v>
       </c>
       <c r="C51">
-        <v>0.2</v>
+        <v>0.75</v>
       </c>
       <c r="D51">
-        <v>0.181818181818</v>
+        <v>0.68181818181800002</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51">
-        <v>2.4642630869</v>
+        <v>22.399506517700001</v>
       </c>
       <c r="G51">
-        <v>6.1024847484799999E-2</v>
+        <v>1.4634587241399999</v>
       </c>
       <c r="T51" s="1" t="s">
         <v>3</v>
@@ -6536,14 +6851,74 @@
       <c r="A62" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C62">
+        <v>0.75</v>
+      </c>
+      <c r="D62">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G62">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="AB62" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="AD62">
+        <v>1</v>
+      </c>
+      <c r="AE62">
+        <v>0.90909090909099999</v>
+      </c>
+      <c r="AF62">
+        <v>1</v>
+      </c>
+      <c r="AG62">
+        <v>34.275829057000003</v>
+      </c>
+      <c r="AH62">
+        <v>1.46345872806</v>
+      </c>
       <c r="AK62" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AM62">
+        <v>1</v>
+      </c>
+      <c r="AN62">
+        <v>0.90909090909099999</v>
+      </c>
+      <c r="AO62">
+        <v>1</v>
+      </c>
+      <c r="AP62">
+        <v>32.283595263400002</v>
+      </c>
+      <c r="AQ62">
+        <v>1.46345872806</v>
+      </c>
       <c r="AT62" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="AV62">
+        <v>0.8</v>
+      </c>
+      <c r="AW62">
+        <v>0.72727272727299996</v>
+      </c>
+      <c r="AX62">
+        <v>1</v>
+      </c>
+      <c r="AY62">
+        <v>24.2238668516</v>
+      </c>
+      <c r="AZ62">
+        <v>1.4634585738500001</v>
       </c>
     </row>
     <row r="63" spans="1:52" x14ac:dyDescent="0.2">
@@ -6921,19 +7296,19 @@
         <v>5</v>
       </c>
       <c r="C68">
-        <v>0.2</v>
+        <v>0.75</v>
       </c>
       <c r="D68">
-        <v>0.181818181818</v>
+        <v>0.68181818181800002</v>
       </c>
       <c r="E68">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="F68">
-        <v>1.0727649539399999</v>
+        <v>22.399506517700001</v>
       </c>
       <c r="G68">
-        <v>1.0023097502899999E-2</v>
+        <v>1.4634587241399999</v>
       </c>
       <c r="AC68" s="1" t="s">
         <v>5</v>
@@ -7512,14 +7887,74 @@
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C76">
+        <v>0.75</v>
+      </c>
+      <c r="D76">
+        <v>0.68181818181800002</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>22.399506517700001</v>
+      </c>
+      <c r="G76">
+        <v>1.4634587241399999</v>
+      </c>
       <c r="AB76" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="AD76">
+        <v>1</v>
+      </c>
+      <c r="AE76">
+        <v>0.90909090909099999</v>
+      </c>
+      <c r="AF76">
+        <v>1</v>
+      </c>
+      <c r="AG76">
+        <v>35.201341909600004</v>
+      </c>
+      <c r="AH76">
+        <v>1.46345872806</v>
+      </c>
       <c r="AK76" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="AM76">
+        <v>0.25</v>
+      </c>
+      <c r="AN76">
+        <v>0.22727272727299999</v>
+      </c>
+      <c r="AO76">
+        <v>0.2</v>
+      </c>
+      <c r="AP76">
+        <v>1.3211226490300001</v>
+      </c>
+      <c r="AQ76">
+        <v>1.26767406359E-2</v>
+      </c>
       <c r="AT76" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="AV76">
+        <v>1</v>
+      </c>
+      <c r="AW76">
+        <v>0.90909090909099999</v>
+      </c>
+      <c r="AX76">
+        <v>1</v>
+      </c>
+      <c r="AY76">
+        <v>10.5056230497</v>
+      </c>
+      <c r="AZ76">
+        <v>0.52811091561800005</v>
       </c>
     </row>
     <row r="77" spans="1:52" x14ac:dyDescent="0.2">
@@ -7527,19 +7962,19 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="D77">
-        <v>0.86363636363600005</v>
+        <v>0.68181818181800002</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77">
-        <v>29.036159929</v>
+        <v>22.399506517700001</v>
       </c>
       <c r="G77">
-        <v>1.46345872806</v>
+        <v>1.4634587241399999</v>
       </c>
       <c r="AC77" s="1" t="s">
         <v>0</v>

</xml_diff>